<commit_message>
Fix Excel file loading - skip first 4 rows, use columns directly
Updated load_test_data.py to properly handle Excel file format:
- Skip first 4 rows (skiprows=4, header=None)
- First column = x-axis (time)
- Second column = y-axis (pressure)
- Removed auto-detection logic - now directly uses column indices
- Added traceback output for better error debugging

Updated test file demo/data/测试数据_NC50.xlsx with 4 header rows to match expected format.

This fixes the loading error when uploading .xlsx files in PT曲线对比 tab.

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/demo/data/测试数据_NC50.xlsx
+++ b/demo/data/测试数据_NC50.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,342 +422,378 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
-          <t>时间</t>
+          <t>Header Row 1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
-          <t>压力</t>
+          <t>Info1</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Header Row 2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Info2</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2.2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Header Row 3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Info3</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4.4</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Header Row 4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Info4</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>6.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>8.800000000000001</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="n">
-        <v>20.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" t="n">
-        <v>39.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" t="n">
-        <v>49</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" t="n">
-        <v>58.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="n">
-        <v>58.2</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>57.9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>57.6</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="n">
-        <v>57.3</v>
+        <v>58.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" t="n">
-        <v>55.5</v>
+        <v>57.9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" t="n">
-        <v>54.3</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" t="n">
-        <v>53.1</v>
+        <v>57.3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" t="n">
-        <v>51.9</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" t="n">
-        <v>50.7</v>
+        <v>54.3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" t="n">
-        <v>49.5</v>
+        <v>53.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" t="n">
-        <v>48.3</v>
+        <v>51.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" t="n">
-        <v>47.1</v>
+        <v>50.7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" t="n">
-        <v>45.9</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" t="n">
-        <v>44.7</v>
+        <v>48.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" t="n">
-        <v>43.5</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" t="n">
-        <v>42.3</v>
+        <v>45.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" t="n">
-        <v>41.1</v>
+        <v>44.7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" t="n">
-        <v>39.9</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" t="n">
-        <v>38.7</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" t="n">
-        <v>37.5</v>
+        <v>41.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33" t="n">
-        <v>36.3</v>
+        <v>39.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" t="n">
-        <v>35.1</v>
+        <v>38.7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B35" t="n">
-        <v>33.9</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" t="n">
-        <v>32.7</v>
+        <v>36.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" t="n">
-        <v>31.5</v>
+        <v>35.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38" t="n">
-        <v>30.3</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B39" t="n">
-        <v>29.1</v>
+        <v>32.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" t="n">
-        <v>27.9</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" t="n">
-        <v>26.7</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
+        <v>37</v>
+      </c>
+      <c r="B42" t="n">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>38</v>
+      </c>
+      <c r="B43" t="n">
+        <v>27.9</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>39</v>
+      </c>
+      <c r="B44" t="n">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B45" t="n">
         <v>25.5</v>
       </c>
     </row>

</xml_diff>